<commit_message>
Last committ on 27/03/2021 At 05:05PM
</commit_message>
<xml_diff>
--- a/PractoAutomation/TestData/Output.xlsx
+++ b/PractoAutomation/TestData/Output.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hxtreme\git\repository3\PractoAutomation\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="10755" windowWidth="24105" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="10755" windowWidth="24105" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="hospitalList" r:id="rId1" sheetId="1"/>
     <sheet name="topCities" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:X33"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="28">
   <si>
     <t>Motherhood Hospital</t>
   </si>
@@ -108,6 +112,9 @@
   </si>
   <si>
     <t>Ahmedabad</t>
+  </si>
+  <si>
+    <t>Queens Hospital</t>
   </si>
 </sst>
 </file>
@@ -462,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>